<commit_message>
Edited volumetric water content calculation and parameter file
</commit_message>
<xml_diff>
--- a/docs/source/tutorials/GenVeg/GenVeg_Dune_Simulation.xlsx
+++ b/docs/source/tutorials/GenVeg/GenVeg_Dune_Simulation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\landlab\docs\source\tutorials\GenVeg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8E929A-DA19-48A5-B72F-272ADCD1ADFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437FDBEA-41BB-47DC-A1D1-65C1615A4D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
+    <workbookView xWindow="45972" yWindow="180" windowWidth="46296" windowHeight="25416" activeTab="1" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -1499,22 +1499,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59430052-850A-4E52-8B29-0C7825B169C3}">
   <dimension ref="A1:K248"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90:D93"/>
+    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="54" style="23" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="23" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="24" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="64.140625" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" style="24" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="64.109375" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>perennial deciduous</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>Poorter</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>Martinez-Vilalta</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>min-max</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>57</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>58</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>17</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
         <v>80</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>19</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>143</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
         <v>66</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
         <v>125</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>23</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>127</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A19" s="28" t="s">
         <v>168</v>
       </c>
@@ -1916,7 +1916,7 @@
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="15">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -1925,7 +1925,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
         <v>162</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
         <v>152</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
         <v>170</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="29" t="s">
         <v>155</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="29" t="s">
         <v>159</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="30" t="s">
         <v>167</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
         <v>158</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A27" s="36" t="s">
         <v>25</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="37"/>
       <c r="B28" s="9" t="s">
         <v>75</v>
@@ -2117,7 +2117,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="37"/>
       <c r="B29" s="9" t="s">
         <v>75</v>
@@ -2138,7 +2138,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="25"/>
       <c r="B30" s="9" t="s">
         <v>75</v>
@@ -2159,7 +2159,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="37" t="s">
         <v>26</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="37"/>
       <c r="B32" s="9" t="s">
         <v>75</v>
@@ -2203,7 +2203,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="37"/>
       <c r="B33" s="9" t="s">
         <v>75</v>
@@ -2224,7 +2224,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="37"/>
       <c r="B34" s="9" t="s">
         <v>75</v>
@@ -2245,7 +2245,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="5" t="s">
         <v>132</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A36" s="36" t="s">
         <v>28</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="37"/>
       <c r="B37" s="9" t="s">
         <v>75</v>
@@ -2305,7 +2305,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="37"/>
       <c r="B38" s="9" t="s">
         <v>75</v>
@@ -2324,7 +2324,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="37"/>
       <c r="B39" s="9" t="s">
         <v>75</v>
@@ -2343,7 +2343,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="37"/>
       <c r="B40" s="9" t="s">
         <v>75</v>
@@ -2362,7 +2362,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="37"/>
       <c r="B41" s="9" t="s">
         <v>75</v>
@@ -2381,7 +2381,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="37"/>
       <c r="B42" s="9" t="s">
         <v>75</v>
@@ -2400,7 +2400,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="35" t="s">
         <v>33</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="35"/>
       <c r="B44" s="9" t="s">
         <v>75</v>
@@ -2444,7 +2444,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="35"/>
       <c r="B45" s="9" t="s">
         <v>75</v>
@@ -2465,7 +2465,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="26"/>
       <c r="B46" s="9" t="s">
         <v>75</v>
@@ -2486,7 +2486,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="35" t="s">
         <v>62</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="35"/>
       <c r="B48" s="9" t="s">
         <v>75</v>
@@ -2530,7 +2530,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="35"/>
       <c r="B49" s="9" t="s">
         <v>75</v>
@@ -2551,7 +2551,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="35"/>
       <c r="B50" s="9" t="s">
         <v>75</v>
@@ -2572,7 +2572,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="31" t="s">
         <v>180</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="35" t="s">
         <v>138</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="35"/>
       <c r="B53" s="9" t="s">
         <v>75</v>
@@ -2639,7 +2639,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="35"/>
       <c r="B54" s="9" t="s">
         <v>75</v>
@@ -2661,7 +2661,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="35"/>
       <c r="B55" s="9" t="s">
         <v>75</v>
@@ -2683,7 +2683,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="35" t="s">
         <v>139</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="35"/>
       <c r="B57" s="9" t="s">
         <v>75</v>
@@ -2729,7 +2729,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="35"/>
       <c r="B58" s="9" t="s">
         <v>75</v>
@@ -2751,7 +2751,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="35"/>
       <c r="B59" s="9" t="s">
         <v>75</v>
@@ -2773,7 +2773,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="35" t="s">
         <v>140</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="35"/>
       <c r="B61" s="9" t="s">
         <v>75</v>
@@ -2819,7 +2819,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="35"/>
       <c r="B62" s="9" t="s">
         <v>75</v>
@@ -2841,7 +2841,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="35"/>
       <c r="B63" s="9" t="s">
         <v>75</v>
@@ -2863,7 +2863,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="35" t="s">
         <v>141</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="35"/>
       <c r="B65" s="9" t="s">
         <v>75</v>
@@ -2909,7 +2909,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="35"/>
       <c r="B66" s="9" t="s">
         <v>75</v>
@@ -2931,7 +2931,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="35"/>
       <c r="B67" s="9" t="s">
         <v>75</v>
@@ -2953,7 +2953,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="5" t="s">
         <v>99</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A69" s="19" t="s">
         <v>35</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="19" t="s">
         <v>37</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="19" t="s">
         <v>181</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="19" t="s">
         <v>106</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="19" t="s">
         <v>101</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="19" t="s">
         <v>171</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="19" t="s">
         <v>112</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="19" t="s">
         <v>103</v>
       </c>
@@ -3144,7 +3144,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="19" t="s">
         <v>114</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="19" t="s">
         <v>116</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="19" t="s">
         <v>173</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="19" t="s">
         <v>117</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="19" t="s">
         <v>119</v>
       </c>
@@ -3249,7 +3249,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="35" t="s">
         <v>186</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="35"/>
       <c r="B83" s="19" t="s">
         <v>76</v>
@@ -3289,7 +3289,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="35" t="s">
         <v>188</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="35"/>
       <c r="B85" s="19" t="s">
         <v>76</v>
@@ -3329,7 +3329,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="35" t="s">
         <v>189</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="35"/>
       <c r="B87" s="19" t="s">
         <v>76</v>
@@ -3369,7 +3369,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="35"/>
       <c r="B88" s="19" t="s">
         <v>76</v>
@@ -3388,7 +3388,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A89" s="19" t="s">
         <v>145</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="35" t="s">
         <v>130</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="35"/>
       <c r="B91" s="19" t="s">
         <v>76</v>
@@ -3456,7 +3456,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="35"/>
       <c r="B92" s="19" t="s">
         <v>76</v>
@@ -3477,7 +3477,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="35"/>
       <c r="B93" s="19" t="s">
         <v>76</v>
@@ -3498,7 +3498,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="19" t="s">
         <v>147</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="5" t="s">
         <v>65</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A96" s="19" t="s">
         <v>107</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="19" t="s">
         <v>108</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="19" t="s">
         <v>109</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="5" t="s">
         <v>39</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A100" s="19" t="s">
         <v>40</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="19" t="s">
         <v>42</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="5" t="s">
         <v>44</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A103" s="19" t="s">
         <v>46</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="19" t="s">
         <v>48</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="19" t="s">
         <v>90</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="19" t="s">
         <v>49</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="19"/>
       <c r="B107" s="19" t="s">
         <v>82</v>
@@ -3797,7 +3797,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="19"/>
       <c r="B108" s="19" t="s">
         <v>82</v>
@@ -3818,7 +3818,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="19"/>
       <c r="B109" s="19" t="s">
         <v>82</v>
@@ -3839,7 +3839,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="19"/>
       <c r="B110" s="19" t="s">
         <v>82</v>
@@ -3858,7 +3858,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="19" t="s">
         <v>96</v>
       </c>
@@ -3881,7 +3881,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="19" t="s">
         <v>97</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="19" t="s">
         <v>98</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="19"/>
       <c r="B114" s="19" t="s">
         <v>82</v>
@@ -3945,7 +3945,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="19"/>
       <c r="B115" s="19" t="s">
         <v>82</v>
@@ -3964,7 +3964,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="19" t="s">
         <v>51</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="19" t="s">
         <v>52</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="19" t="s">
         <v>93</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="19" t="s">
         <v>53</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="19"/>
       <c r="B120" s="19" t="s">
         <v>82</v>
@@ -4077,7 +4077,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="19"/>
       <c r="B121" s="19" t="s">
         <v>82</v>
@@ -4098,7 +4098,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="19"/>
       <c r="B122" s="19" t="s">
         <v>82</v>
@@ -4119,7 +4119,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="19"/>
       <c r="B123" s="19" t="s">
         <v>82</v>
@@ -4140,7 +4140,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="19" t="s">
         <v>54</v>
       </c>
@@ -4163,7 +4163,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="19" t="s">
         <v>97</v>
       </c>
@@ -4183,7 +4183,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="19" t="s">
         <v>98</v>
       </c>
@@ -4203,7 +4203,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="19"/>
       <c r="B127" s="19" t="s">
         <v>82</v>
@@ -4221,7 +4221,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="19"/>
       <c r="B128" s="19" t="s">
         <v>82</v>
@@ -4239,7 +4239,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="19" t="s">
         <v>198</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="19" t="s">
         <v>200</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="19" t="s">
         <v>201</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="19" t="s">
         <v>199</v>
       </c>
@@ -4307,7 +4307,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="19"/>
       <c r="B133" s="19" t="s">
         <v>82</v>
@@ -4322,7 +4322,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="19"/>
       <c r="B134" s="19" t="s">
         <v>82</v>
@@ -4337,7 +4337,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="19"/>
       <c r="B135" s="19" t="s">
         <v>82</v>
@@ -4352,7 +4352,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" s="19"/>
       <c r="B136" s="19" t="s">
         <v>82</v>
@@ -4367,7 +4367,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="19" t="s">
         <v>202</v>
       </c>
@@ -4384,7 +4384,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="19" t="s">
         <v>97</v>
       </c>
@@ -4401,7 +4401,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="19" t="s">
         <v>98</v>
       </c>
@@ -4418,7 +4418,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="19"/>
       <c r="B140" s="19" t="s">
         <v>82</v>
@@ -4433,7 +4433,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" s="19"/>
       <c r="B141" s="19" t="s">
         <v>82</v>
@@ -4448,7 +4448,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="19" t="s">
         <v>203</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" s="19" t="s">
         <v>205</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" s="19" t="s">
         <v>206</v>
       </c>
@@ -4499,7 +4499,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" s="19" t="s">
         <v>204</v>
       </c>
@@ -4516,7 +4516,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" s="19"/>
       <c r="B146" s="19" t="s">
         <v>82</v>
@@ -4531,7 +4531,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" s="19"/>
       <c r="B147" s="19" t="s">
         <v>82</v>
@@ -4546,7 +4546,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" s="19"/>
       <c r="B148" s="19" t="s">
         <v>82</v>
@@ -4561,7 +4561,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" s="19"/>
       <c r="B149" s="19" t="s">
         <v>82</v>
@@ -4576,7 +4576,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" s="19" t="s">
         <v>207</v>
       </c>
@@ -4593,7 +4593,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" s="19" t="s">
         <v>97</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" s="19" t="s">
         <v>98</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" s="19"/>
       <c r="B153" s="19" t="s">
         <v>82</v>
@@ -4642,7 +4642,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" s="19"/>
       <c r="B154" s="19" t="s">
         <v>82</v>
@@ -4657,7 +4657,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" s="19" t="s">
         <v>209</v>
       </c>
@@ -4674,7 +4674,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" s="19" t="s">
         <v>208</v>
       </c>
@@ -4691,7 +4691,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" s="19" t="s">
         <v>210</v>
       </c>
@@ -4708,7 +4708,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" s="19" t="s">
         <v>211</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" s="19"/>
       <c r="B159" s="19" t="s">
         <v>82</v>
@@ -4740,7 +4740,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" s="19"/>
       <c r="B160" s="19" t="s">
         <v>82</v>
@@ -4755,7 +4755,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" s="19"/>
       <c r="B161" s="19" t="s">
         <v>82</v>
@@ -4770,7 +4770,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" s="19"/>
       <c r="B162" s="19" t="s">
         <v>82</v>
@@ -4785,7 +4785,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" s="19" t="s">
         <v>212</v>
       </c>
@@ -4802,7 +4802,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" s="19" t="s">
         <v>97</v>
       </c>
@@ -4819,7 +4819,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" s="19" t="s">
         <v>98</v>
       </c>
@@ -4836,7 +4836,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" s="19"/>
       <c r="B166" s="19" t="s">
         <v>82</v>
@@ -4851,7 +4851,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" s="19"/>
       <c r="B167" s="19" t="s">
         <v>82</v>
@@ -4866,489 +4866,484 @@
         <v>179</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" s="20"/>
       <c r="B168" s="20"/>
       <c r="C168" s="21"/>
       <c r="D168" s="22"/>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="20"/>
       <c r="B169" s="20"/>
       <c r="C169" s="21"/>
       <c r="D169" s="22"/>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" s="20"/>
       <c r="B170" s="20"/>
       <c r="C170" s="21"/>
       <c r="D170" s="22"/>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" s="20"/>
       <c r="B171" s="20"/>
       <c r="C171" s="21"/>
       <c r="D171" s="22"/>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" s="20"/>
       <c r="B172" s="20"/>
       <c r="C172" s="21"/>
       <c r="D172" s="22"/>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173" s="20"/>
       <c r="B173" s="20"/>
       <c r="C173" s="21"/>
       <c r="D173" s="22"/>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" s="20"/>
       <c r="B174" s="20"/>
       <c r="C174" s="21"/>
       <c r="D174" s="22"/>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" s="20"/>
       <c r="B175" s="20"/>
       <c r="C175" s="21"/>
       <c r="D175" s="22"/>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176" s="20"/>
       <c r="B176" s="20"/>
       <c r="C176" s="21"/>
       <c r="D176" s="22"/>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="20"/>
       <c r="B177" s="20"/>
       <c r="C177" s="21"/>
       <c r="D177" s="22"/>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="20"/>
       <c r="B178" s="20"/>
       <c r="C178" s="21"/>
       <c r="D178" s="22"/>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="20"/>
       <c r="B179" s="20"/>
       <c r="C179" s="21"/>
       <c r="D179" s="22"/>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="20"/>
       <c r="B180" s="20"/>
       <c r="C180" s="21"/>
       <c r="D180" s="22"/>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="20"/>
       <c r="B181" s="20"/>
       <c r="C181" s="21"/>
       <c r="D181" s="22"/>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="20"/>
       <c r="B182" s="20"/>
       <c r="C182" s="21"/>
       <c r="D182" s="22"/>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="20"/>
       <c r="B183" s="20"/>
       <c r="C183" s="21"/>
       <c r="D183" s="22"/>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="20"/>
       <c r="B184" s="20"/>
       <c r="C184" s="21"/>
       <c r="D184" s="22"/>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="20"/>
       <c r="B185" s="20"/>
       <c r="C185" s="21"/>
       <c r="D185" s="22"/>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="20"/>
       <c r="B186" s="20"/>
       <c r="C186" s="21"/>
       <c r="D186" s="22"/>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" s="20"/>
       <c r="B187" s="20"/>
       <c r="C187" s="21"/>
       <c r="D187" s="22"/>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="20"/>
       <c r="B188" s="20"/>
       <c r="C188" s="21"/>
       <c r="D188" s="22"/>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="20"/>
       <c r="B189" s="20"/>
       <c r="C189" s="21"/>
       <c r="D189" s="22"/>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="20"/>
       <c r="B190" s="20"/>
       <c r="C190" s="21"/>
       <c r="D190" s="22"/>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="20"/>
       <c r="B191" s="20"/>
       <c r="C191" s="21"/>
       <c r="D191" s="22"/>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="20"/>
       <c r="B192" s="20"/>
       <c r="C192" s="21"/>
       <c r="D192" s="22"/>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" s="20"/>
       <c r="B193" s="20"/>
       <c r="C193" s="21"/>
       <c r="D193" s="22"/>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="20"/>
       <c r="B194" s="20"/>
       <c r="C194" s="21"/>
       <c r="D194" s="22"/>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="20"/>
       <c r="B195" s="20"/>
       <c r="C195" s="21"/>
       <c r="D195" s="22"/>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="20"/>
       <c r="B196" s="20"/>
       <c r="C196" s="21"/>
       <c r="D196" s="22"/>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" s="20"/>
       <c r="B197" s="20"/>
       <c r="C197" s="21"/>
       <c r="D197" s="22"/>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" s="20"/>
       <c r="B198" s="20"/>
       <c r="C198" s="21"/>
       <c r="D198" s="22"/>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="20"/>
       <c r="B199" s="20"/>
       <c r="C199" s="21"/>
       <c r="D199" s="22"/>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" s="20"/>
       <c r="B200" s="20"/>
       <c r="C200" s="21"/>
       <c r="D200" s="22"/>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" s="20"/>
       <c r="B201" s="20"/>
       <c r="C201" s="21"/>
       <c r="D201" s="22"/>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" s="20"/>
       <c r="B202" s="20"/>
       <c r="C202" s="21"/>
       <c r="D202" s="22"/>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" s="20"/>
       <c r="B203" s="20"/>
       <c r="C203" s="21"/>
       <c r="D203" s="22"/>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" s="20"/>
       <c r="B204" s="20"/>
       <c r="C204" s="21"/>
       <c r="D204" s="22"/>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" s="20"/>
       <c r="B205" s="20"/>
       <c r="C205" s="21"/>
       <c r="D205" s="22"/>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" s="20"/>
       <c r="B206" s="20"/>
       <c r="C206" s="21"/>
       <c r="D206" s="22"/>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" s="20"/>
       <c r="B207" s="20"/>
       <c r="C207" s="21"/>
       <c r="D207" s="22"/>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" s="20"/>
       <c r="B208" s="20"/>
       <c r="C208" s="21"/>
       <c r="D208" s="22"/>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" s="20"/>
       <c r="B209" s="20"/>
       <c r="C209" s="21"/>
       <c r="D209" s="22"/>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" s="20"/>
       <c r="B210" s="20"/>
       <c r="C210" s="21"/>
       <c r="D210" s="22"/>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="20"/>
       <c r="B211" s="20"/>
       <c r="C211" s="21"/>
       <c r="D211" s="22"/>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="20"/>
       <c r="B212" s="20"/>
       <c r="C212" s="21"/>
       <c r="D212" s="22"/>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="20"/>
       <c r="B213" s="20"/>
       <c r="C213" s="21"/>
       <c r="D213" s="22"/>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" s="20"/>
       <c r="B214" s="20"/>
       <c r="C214" s="21"/>
       <c r="D214" s="22"/>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" s="20"/>
       <c r="B215" s="20"/>
       <c r="C215" s="21"/>
       <c r="D215" s="22"/>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" s="20"/>
       <c r="B216" s="20"/>
       <c r="C216" s="21"/>
       <c r="D216" s="22"/>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" s="20"/>
       <c r="B217" s="20"/>
       <c r="C217" s="21"/>
       <c r="D217" s="22"/>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" s="20"/>
       <c r="B218" s="20"/>
       <c r="C218" s="21"/>
       <c r="D218" s="22"/>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" s="20"/>
       <c r="B219" s="20"/>
       <c r="C219" s="21"/>
       <c r="D219" s="22"/>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" s="20"/>
       <c r="B220" s="20"/>
       <c r="C220" s="21"/>
       <c r="D220" s="22"/>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" s="20"/>
       <c r="B221" s="20"/>
       <c r="C221" s="21"/>
       <c r="D221" s="22"/>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" s="20"/>
       <c r="B222" s="20"/>
       <c r="C222" s="21"/>
       <c r="D222" s="22"/>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" s="20"/>
       <c r="B223" s="20"/>
       <c r="C223" s="21"/>
       <c r="D223" s="22"/>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" s="20"/>
       <c r="B224" s="20"/>
       <c r="C224" s="21"/>
       <c r="D224" s="22"/>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" s="20"/>
       <c r="B225" s="20"/>
       <c r="C225" s="21"/>
       <c r="D225" s="22"/>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" s="20"/>
       <c r="B226" s="20"/>
       <c r="C226" s="21"/>
       <c r="D226" s="22"/>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" s="20"/>
       <c r="B227" s="20"/>
       <c r="C227" s="21"/>
       <c r="D227" s="22"/>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" s="20"/>
       <c r="B228" s="20"/>
       <c r="C228" s="21"/>
       <c r="D228" s="22"/>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" s="20"/>
       <c r="B229" s="20"/>
       <c r="C229" s="21"/>
       <c r="D229" s="22"/>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" s="20"/>
       <c r="B230" s="20"/>
       <c r="C230" s="21"/>
       <c r="D230" s="22"/>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" s="20"/>
       <c r="B231" s="20"/>
       <c r="C231" s="21"/>
       <c r="D231" s="22"/>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" s="20"/>
       <c r="B232" s="20"/>
       <c r="C232" s="21"/>
       <c r="D232" s="22"/>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" s="20"/>
       <c r="B233" s="20"/>
       <c r="C233" s="21"/>
       <c r="D233" s="22"/>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" s="20"/>
       <c r="B234" s="20"/>
       <c r="C234" s="21"/>
       <c r="D234" s="22"/>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" s="20"/>
       <c r="B235" s="20"/>
       <c r="C235" s="21"/>
       <c r="D235" s="22"/>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" s="20"/>
       <c r="B236" s="20"/>
       <c r="C236" s="21"/>
       <c r="D236" s="22"/>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" s="20"/>
       <c r="B237" s="20"/>
       <c r="C237" s="21"/>
       <c r="D237" s="22"/>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" s="20"/>
       <c r="B238" s="20"/>
       <c r="C238" s="21"/>
       <c r="D238" s="22"/>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" s="20"/>
       <c r="C239" s="21"/>
       <c r="D239" s="22"/>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" s="20"/>
       <c r="C240" s="21"/>
       <c r="D240" s="22"/>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" s="20"/>
       <c r="C241" s="21"/>
       <c r="D241" s="22"/>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" s="20"/>
       <c r="C242" s="21"/>
       <c r="D242" s="22"/>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" s="20"/>
       <c r="C243" s="21"/>
       <c r="D243" s="22"/>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" s="20"/>
       <c r="C244" s="21"/>
       <c r="D244" s="22"/>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" s="20"/>
       <c r="C245" s="21"/>
       <c r="D245" s="22"/>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" s="20"/>
       <c r="C246" s="21"/>
       <c r="D246" s="22"/>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" s="20"/>
       <c r="C247" s="21"/>
       <c r="D247" s="22"/>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" s="20"/>
       <c r="C248" s="21"/>
       <c r="D248" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="A86:A88"/>
-    <mergeCell ref="A90:A93"/>
-    <mergeCell ref="A64:A67"/>
     <mergeCell ref="A52:A55"/>
     <mergeCell ref="A56:A59"/>
     <mergeCell ref="A60:A63"/>
@@ -5357,6 +5352,11 @@
     <mergeCell ref="A36:A42"/>
     <mergeCell ref="A47:A50"/>
     <mergeCell ref="A43:A45"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="A86:A88"/>
+    <mergeCell ref="A90:A93"/>
+    <mergeCell ref="A64:A67"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="20">
@@ -5437,22 +5437,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5B2ED1-E60A-481E-A183-520033C5AF7F}">
   <dimension ref="A1:N248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.140625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="23" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="24" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="64.140625" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="41.109375" style="23" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" style="24" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="64.109375" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -5500,7 +5500,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -5525,7 +5525,7 @@
         <v>perennial deciduous</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -5550,7 +5550,7 @@
         <v>Poorter</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -5575,7 +5575,7 @@
         <v>Martinez-Vilalta</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
@@ -5596,7 +5596,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>57</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>58</v>
       </c>
@@ -5638,7 +5638,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>17</v>
       </c>
@@ -5659,7 +5659,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
         <v>80</v>
       </c>
@@ -5675,7 +5675,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>19</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
@@ -5717,7 +5717,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>143</v>
       </c>
@@ -5738,7 +5738,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
         <v>66</v>
       </c>
@@ -5759,7 +5759,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
         <v>125</v>
       </c>
@@ -5780,7 +5780,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>23</v>
       </c>
@@ -5801,7 +5801,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>127</v>
       </c>
@@ -5822,7 +5822,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
@@ -5838,7 +5838,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A19" s="28" t="s">
         <v>150</v>
       </c>
@@ -5850,7 +5850,7 @@
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="15">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F19" t="s">
         <v>161</v>
@@ -5862,7 +5862,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="28" t="s">
         <v>162</v>
       </c>
@@ -5883,7 +5883,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="28" t="s">
         <v>152</v>
       </c>
@@ -5904,7 +5904,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="28" t="s">
         <v>163</v>
       </c>
@@ -5925,7 +5925,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="28" t="s">
         <v>155</v>
       </c>
@@ -5946,7 +5946,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>159</v>
       </c>
@@ -5967,7 +5967,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="30" t="s">
         <v>167</v>
       </c>
@@ -5991,7 +5991,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
         <v>158</v>
       </c>
@@ -6007,7 +6007,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37" t="s">
         <v>25</v>
       </c>
@@ -6030,7 +6030,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="37"/>
       <c r="B28" s="9" t="s">
         <v>75</v>
@@ -6051,7 +6051,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="37"/>
       <c r="B29" s="9" t="s">
         <v>75</v>
@@ -6072,7 +6072,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="37"/>
       <c r="B30" s="9" t="s">
         <v>75</v>
@@ -6093,7 +6093,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="37" t="s">
         <v>26</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="37"/>
       <c r="B32" s="9" t="s">
         <v>75</v>
@@ -6137,7 +6137,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="37"/>
       <c r="B33" s="9" t="s">
         <v>75</v>
@@ -6158,7 +6158,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="37"/>
       <c r="B34" s="9" t="s">
         <v>75</v>
@@ -6179,7 +6179,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="5" t="s">
         <v>132</v>
       </c>
@@ -6195,7 +6195,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A36" s="34"/>
       <c r="B36" s="33" t="s">
         <v>75</v>
@@ -6217,7 +6217,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="39" t="s">
         <v>28</v>
       </c>
@@ -6241,7 +6241,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="39"/>
       <c r="B38" s="9" t="s">
         <v>75</v>
@@ -6261,7 +6261,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="39"/>
       <c r="B39" s="9" t="s">
         <v>75</v>
@@ -6281,7 +6281,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="39"/>
       <c r="B40" s="9" t="s">
         <v>75</v>
@@ -6301,7 +6301,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="39"/>
       <c r="B41" s="9" t="s">
         <v>75</v>
@@ -6321,7 +6321,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="39"/>
       <c r="B42" s="9" t="s">
         <v>75</v>
@@ -6341,7 +6341,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="35" t="s">
         <v>33</v>
       </c>
@@ -6364,7 +6364,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="35"/>
       <c r="B44" s="9" t="s">
         <v>75</v>
@@ -6386,7 +6386,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="35"/>
       <c r="B45" s="9" t="s">
         <v>75</v>
@@ -6407,7 +6407,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="35"/>
       <c r="B46" s="9" t="s">
         <v>75</v>
@@ -6428,7 +6428,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="35" t="s">
         <v>62</v>
       </c>
@@ -6451,7 +6451,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="35"/>
       <c r="B48" s="9" t="s">
         <v>75</v>
@@ -6480,7 +6480,7 @@
         <v>0.3979400086720376</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="35"/>
       <c r="B49" s="9" t="s">
         <v>75</v>
@@ -6509,7 +6509,7 @@
         <v>1.5740312677277188</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="35"/>
       <c r="B50" s="9" t="s">
         <v>75</v>
@@ -6530,7 +6530,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="32" t="s">
         <v>180</v>
       </c>
@@ -6551,7 +6551,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="35" t="s">
         <v>138</v>
       </c>
@@ -6575,7 +6575,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="35"/>
       <c r="B53" s="9" t="s">
         <v>75</v>
@@ -6597,7 +6597,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="35"/>
       <c r="B54" s="9" t="s">
         <v>75</v>
@@ -6619,7 +6619,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="35"/>
       <c r="B55" s="9" t="s">
         <v>75</v>
@@ -6641,7 +6641,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="35" t="s">
         <v>139</v>
       </c>
@@ -6665,7 +6665,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="35"/>
       <c r="B57" s="9" t="s">
         <v>75</v>
@@ -6687,7 +6687,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="35"/>
       <c r="B58" s="9" t="s">
         <v>75</v>
@@ -6709,7 +6709,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="35"/>
       <c r="B59" s="9" t="s">
         <v>75</v>
@@ -6731,7 +6731,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="35" t="s">
         <v>140</v>
       </c>
@@ -6755,7 +6755,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="35"/>
       <c r="B61" s="9" t="s">
         <v>75</v>
@@ -6777,7 +6777,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="35"/>
       <c r="B62" s="9" t="s">
         <v>75</v>
@@ -6799,7 +6799,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="35"/>
       <c r="B63" s="9" t="s">
         <v>75</v>
@@ -6821,7 +6821,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="35" t="s">
         <v>141</v>
       </c>
@@ -6845,7 +6845,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="35"/>
       <c r="B65" s="9" t="s">
         <v>75</v>
@@ -6867,7 +6867,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="35"/>
       <c r="B66" s="9" t="s">
         <v>75</v>
@@ -6889,7 +6889,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="35"/>
       <c r="B67" s="9" t="s">
         <v>75</v>
@@ -6911,7 +6911,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="5" t="s">
         <v>99</v>
       </c>
@@ -6927,7 +6927,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A69" s="19" t="s">
         <v>35</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="19" t="s">
         <v>37</v>
       </c>
@@ -6969,7 +6969,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="19" t="s">
         <v>181</v>
       </c>
@@ -6993,7 +6993,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="19" t="s">
         <v>106</v>
       </c>
@@ -7014,7 +7014,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="19" t="s">
         <v>101</v>
       </c>
@@ -7035,7 +7035,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="19" t="s">
         <v>171</v>
       </c>
@@ -7056,7 +7056,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="19" t="s">
         <v>102</v>
       </c>
@@ -7077,7 +7077,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="19" t="s">
         <v>103</v>
       </c>
@@ -7098,7 +7098,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="19" t="s">
         <v>114</v>
       </c>
@@ -7124,7 +7124,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="19" t="s">
         <v>116</v>
       </c>
@@ -7145,7 +7145,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="19" t="s">
         <v>173</v>
       </c>
@@ -7166,7 +7166,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="19" t="s">
         <v>117</v>
       </c>
@@ -7187,7 +7187,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="19" t="s">
         <v>119</v>
       </c>
@@ -7208,7 +7208,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="35" t="s">
         <v>186</v>
       </c>
@@ -7229,7 +7229,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="35"/>
       <c r="B83" s="19" t="s">
         <v>76</v>
@@ -7248,7 +7248,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="35" t="s">
         <v>188</v>
       </c>
@@ -7269,7 +7269,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="35"/>
       <c r="B85" s="19" t="s">
         <v>76</v>
@@ -7288,7 +7288,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="35" t="s">
         <v>189</v>
       </c>
@@ -7309,7 +7309,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="35"/>
       <c r="B87" s="19" t="s">
         <v>76</v>
@@ -7328,7 +7328,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="35"/>
       <c r="B88" s="19" t="s">
         <v>76</v>
@@ -7347,7 +7347,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A89" s="19" t="s">
         <v>145</v>
       </c>
@@ -7368,7 +7368,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="19" t="s">
         <v>130</v>
       </c>
@@ -7394,7 +7394,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="19"/>
       <c r="B91" s="19" t="s">
         <v>76</v>
@@ -7415,7 +7415,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="19"/>
       <c r="B92" s="19" t="s">
         <v>76</v>
@@ -7436,7 +7436,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="19"/>
       <c r="B93" s="19" t="s">
         <v>76</v>
@@ -7457,7 +7457,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="19" t="s">
         <v>147</v>
       </c>
@@ -7481,7 +7481,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="5" t="s">
         <v>65</v>
       </c>
@@ -7497,7 +7497,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A96" s="19" t="s">
         <v>107</v>
       </c>
@@ -7518,7 +7518,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="19" t="s">
         <v>108</v>
       </c>
@@ -7539,7 +7539,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="19" t="s">
         <v>109</v>
       </c>
@@ -7560,7 +7560,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="5" t="s">
         <v>39</v>
       </c>
@@ -7578,7 +7578,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A100" s="19" t="s">
         <v>40</v>
       </c>
@@ -7599,7 +7599,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="19" t="s">
         <v>42</v>
       </c>
@@ -7623,7 +7623,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="5" t="s">
         <v>44</v>
       </c>
@@ -7639,7 +7639,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A103" s="19" t="s">
         <v>46</v>
       </c>
@@ -7662,7 +7662,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="19" t="s">
         <v>48</v>
       </c>
@@ -7685,7 +7685,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="19" t="s">
         <v>90</v>
       </c>
@@ -7708,7 +7708,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="19" t="s">
         <v>49</v>
       </c>
@@ -7731,7 +7731,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="19"/>
       <c r="B107" s="19" t="s">
         <v>82</v>
@@ -7752,7 +7752,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="19"/>
       <c r="B108" s="19" t="s">
         <v>82</v>
@@ -7773,7 +7773,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="19"/>
       <c r="B109" s="19" t="s">
         <v>82</v>
@@ -7794,7 +7794,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="19"/>
       <c r="B110" s="19" t="s">
         <v>82</v>
@@ -7813,7 +7813,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="19" t="s">
         <v>50</v>
       </c>
@@ -7836,7 +7836,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="19"/>
       <c r="B112" s="19" t="s">
         <v>82</v>
@@ -7857,7 +7857,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="19"/>
       <c r="B113" s="19" t="s">
         <v>82</v>
@@ -7878,7 +7878,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="19"/>
       <c r="B114" s="19" t="s">
         <v>82</v>
@@ -7902,7 +7902,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="19"/>
       <c r="B115" s="19" t="s">
         <v>82</v>
@@ -7921,7 +7921,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="19" t="s">
         <v>51</v>
       </c>
@@ -7944,7 +7944,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="19" t="s">
         <v>52</v>
       </c>
@@ -7967,7 +7967,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="19" t="s">
         <v>93</v>
       </c>
@@ -7990,7 +7990,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="19" t="s">
         <v>53</v>
       </c>
@@ -8013,7 +8013,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="19"/>
       <c r="B120" s="19" t="s">
         <v>82</v>
@@ -8034,7 +8034,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="19"/>
       <c r="B121" s="19" t="s">
         <v>82</v>
@@ -8055,7 +8055,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="19"/>
       <c r="B122" s="19" t="s">
         <v>82</v>
@@ -8076,7 +8076,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="19"/>
       <c r="B123" s="19" t="s">
         <v>82</v>
@@ -8097,7 +8097,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="19" t="s">
         <v>54</v>
       </c>
@@ -8120,7 +8120,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="19"/>
       <c r="B125" s="19" t="s">
         <v>82</v>
@@ -8141,7 +8141,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="19"/>
       <c r="B126" s="19" t="s">
         <v>82</v>
@@ -8162,7 +8162,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="19"/>
       <c r="B127" s="19" t="s">
         <v>82</v>
@@ -8183,7 +8183,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="19"/>
       <c r="B128" s="19" t="s">
         <v>82</v>
@@ -8204,7 +8204,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="19" t="s">
         <v>198</v>
       </c>
@@ -8224,7 +8224,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="19" t="s">
         <v>200</v>
       </c>
@@ -8244,7 +8244,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="19" t="s">
         <v>201</v>
       </c>
@@ -8264,7 +8264,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="19" t="s">
         <v>199</v>
       </c>
@@ -8284,7 +8284,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="19"/>
       <c r="B133" s="19" t="s">
         <v>82</v>
@@ -8302,7 +8302,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="19"/>
       <c r="B134" s="19" t="s">
         <v>82</v>
@@ -8320,7 +8320,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="19"/>
       <c r="B135" s="19" t="s">
         <v>82</v>
@@ -8338,7 +8338,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" s="19"/>
       <c r="B136" s="19" t="s">
         <v>82</v>
@@ -8356,7 +8356,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="19" t="s">
         <v>202</v>
       </c>
@@ -8376,7 +8376,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="19" t="s">
         <v>97</v>
       </c>
@@ -8396,7 +8396,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="19" t="s">
         <v>98</v>
       </c>
@@ -8416,7 +8416,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="19"/>
       <c r="B140" s="19" t="s">
         <v>82</v>
@@ -8434,7 +8434,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" s="19"/>
       <c r="B141" s="19" t="s">
         <v>82</v>
@@ -8452,7 +8452,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="19" t="s">
         <v>203</v>
       </c>
@@ -8472,7 +8472,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" s="19" t="s">
         <v>205</v>
       </c>
@@ -8492,7 +8492,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" s="19" t="s">
         <v>206</v>
       </c>
@@ -8512,7 +8512,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" s="19" t="s">
         <v>204</v>
       </c>
@@ -8532,7 +8532,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" s="19"/>
       <c r="B146" s="19" t="s">
         <v>82</v>
@@ -8550,7 +8550,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" s="19"/>
       <c r="B147" s="19" t="s">
         <v>82</v>
@@ -8568,7 +8568,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" s="19"/>
       <c r="B148" s="19" t="s">
         <v>82</v>
@@ -8586,7 +8586,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" s="19"/>
       <c r="B149" s="19" t="s">
         <v>82</v>
@@ -8604,7 +8604,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" s="19" t="s">
         <v>207</v>
       </c>
@@ -8624,7 +8624,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" s="19" t="s">
         <v>97</v>
       </c>
@@ -8644,7 +8644,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" s="19" t="s">
         <v>98</v>
       </c>
@@ -8664,7 +8664,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" s="19"/>
       <c r="B153" s="19" t="s">
         <v>82</v>
@@ -8682,7 +8682,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" s="19"/>
       <c r="B154" s="19" t="s">
         <v>82</v>
@@ -8700,7 +8700,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" s="19" t="s">
         <v>209</v>
       </c>
@@ -8720,7 +8720,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" s="19" t="s">
         <v>208</v>
       </c>
@@ -8740,7 +8740,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" s="19" t="s">
         <v>210</v>
       </c>
@@ -8760,7 +8760,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" s="19" t="s">
         <v>211</v>
       </c>
@@ -8780,7 +8780,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" s="19"/>
       <c r="B159" s="19" t="s">
         <v>82</v>
@@ -8798,7 +8798,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" s="19"/>
       <c r="B160" s="19" t="s">
         <v>82</v>
@@ -8816,7 +8816,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" s="19"/>
       <c r="B161" s="19" t="s">
         <v>82</v>
@@ -8834,7 +8834,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" s="19"/>
       <c r="B162" s="19" t="s">
         <v>82</v>
@@ -8852,7 +8852,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" s="19" t="s">
         <v>212</v>
       </c>
@@ -8872,7 +8872,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" s="19" t="s">
         <v>97</v>
       </c>
@@ -8892,7 +8892,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" s="19" t="s">
         <v>98</v>
       </c>
@@ -8912,7 +8912,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" s="19"/>
       <c r="B166" s="19" t="s">
         <v>82</v>
@@ -8930,7 +8930,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" s="19"/>
       <c r="B167" s="19" t="s">
         <v>82</v>
@@ -8948,487 +8948,487 @@
         <v>179</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" s="20"/>
       <c r="B168" s="20"/>
       <c r="C168" s="21"/>
       <c r="D168" s="22"/>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="20"/>
       <c r="B169" s="20"/>
       <c r="C169" s="21"/>
       <c r="D169" s="22"/>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" s="20"/>
       <c r="B170" s="20"/>
       <c r="C170" s="21"/>
       <c r="D170" s="22"/>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" s="20"/>
       <c r="B171" s="20"/>
       <c r="C171" s="21"/>
       <c r="D171" s="22"/>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" s="20"/>
       <c r="B172" s="20"/>
       <c r="C172" s="21"/>
       <c r="D172" s="22"/>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173" s="20"/>
       <c r="B173" s="20"/>
       <c r="C173" s="21"/>
       <c r="D173" s="22"/>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" s="20"/>
       <c r="B174" s="20"/>
       <c r="C174" s="21"/>
       <c r="D174" s="22"/>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" s="20"/>
       <c r="B175" s="20"/>
       <c r="C175" s="21"/>
       <c r="D175" s="22"/>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176" s="20"/>
       <c r="B176" s="20"/>
       <c r="C176" s="21"/>
       <c r="D176" s="22"/>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="20"/>
       <c r="B177" s="20"/>
       <c r="C177" s="21"/>
       <c r="D177" s="22"/>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="20"/>
       <c r="B178" s="20"/>
       <c r="C178" s="21"/>
       <c r="D178" s="22"/>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="20"/>
       <c r="B179" s="20"/>
       <c r="C179" s="21"/>
       <c r="D179" s="22"/>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="20"/>
       <c r="B180" s="20"/>
       <c r="C180" s="21"/>
       <c r="D180" s="22"/>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="20"/>
       <c r="B181" s="20"/>
       <c r="C181" s="21"/>
       <c r="D181" s="22"/>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="20"/>
       <c r="B182" s="20"/>
       <c r="C182" s="21"/>
       <c r="D182" s="22"/>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="20"/>
       <c r="B183" s="20"/>
       <c r="C183" s="21"/>
       <c r="D183" s="22"/>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="20"/>
       <c r="B184" s="20"/>
       <c r="C184" s="21"/>
       <c r="D184" s="22"/>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="20"/>
       <c r="B185" s="20"/>
       <c r="C185" s="21"/>
       <c r="D185" s="22"/>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="20"/>
       <c r="B186" s="20"/>
       <c r="C186" s="21"/>
       <c r="D186" s="22"/>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" s="20"/>
       <c r="B187" s="20"/>
       <c r="C187" s="21"/>
       <c r="D187" s="22"/>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="20"/>
       <c r="B188" s="20"/>
       <c r="C188" s="21"/>
       <c r="D188" s="22"/>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="20"/>
       <c r="B189" s="20"/>
       <c r="C189" s="21"/>
       <c r="D189" s="22"/>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="20"/>
       <c r="B190" s="20"/>
       <c r="C190" s="21"/>
       <c r="D190" s="22"/>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="20"/>
       <c r="B191" s="20"/>
       <c r="C191" s="21"/>
       <c r="D191" s="22"/>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="20"/>
       <c r="B192" s="20"/>
       <c r="C192" s="21"/>
       <c r="D192" s="22"/>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" s="20"/>
       <c r="B193" s="20"/>
       <c r="C193" s="21"/>
       <c r="D193" s="22"/>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="20"/>
       <c r="B194" s="20"/>
       <c r="C194" s="21"/>
       <c r="D194" s="22"/>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="20"/>
       <c r="B195" s="20"/>
       <c r="C195" s="21"/>
       <c r="D195" s="22"/>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="20"/>
       <c r="B196" s="20"/>
       <c r="C196" s="21"/>
       <c r="D196" s="22"/>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" s="20"/>
       <c r="B197" s="20"/>
       <c r="C197" s="21"/>
       <c r="D197" s="22"/>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" s="20"/>
       <c r="B198" s="20"/>
       <c r="C198" s="21"/>
       <c r="D198" s="22"/>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="20"/>
       <c r="B199" s="20"/>
       <c r="C199" s="21"/>
       <c r="D199" s="22"/>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" s="20"/>
       <c r="B200" s="20"/>
       <c r="C200" s="21"/>
       <c r="D200" s="22"/>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" s="20"/>
       <c r="B201" s="20"/>
       <c r="C201" s="21"/>
       <c r="D201" s="22"/>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" s="20"/>
       <c r="B202" s="20"/>
       <c r="C202" s="21"/>
       <c r="D202" s="22"/>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" s="20"/>
       <c r="B203" s="20"/>
       <c r="C203" s="21"/>
       <c r="D203" s="22"/>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" s="20"/>
       <c r="B204" s="20"/>
       <c r="C204" s="21"/>
       <c r="D204" s="22"/>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" s="20"/>
       <c r="B205" s="20"/>
       <c r="C205" s="21"/>
       <c r="D205" s="22"/>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" s="20"/>
       <c r="B206" s="20"/>
       <c r="C206" s="21"/>
       <c r="D206" s="22"/>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" s="20"/>
       <c r="B207" s="20"/>
       <c r="C207" s="21"/>
       <c r="D207" s="22"/>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" s="20"/>
       <c r="B208" s="20"/>
       <c r="C208" s="21"/>
       <c r="D208" s="22"/>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" s="20"/>
       <c r="B209" s="20"/>
       <c r="C209" s="21"/>
       <c r="D209" s="22"/>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" s="20"/>
       <c r="B210" s="20"/>
       <c r="C210" s="21"/>
       <c r="D210" s="22"/>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="20"/>
       <c r="B211" s="20"/>
       <c r="C211" s="21"/>
       <c r="D211" s="22"/>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="20"/>
       <c r="B212" s="20"/>
       <c r="C212" s="21"/>
       <c r="D212" s="22"/>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="20"/>
       <c r="B213" s="20"/>
       <c r="C213" s="21"/>
       <c r="D213" s="22"/>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" s="20"/>
       <c r="B214" s="20"/>
       <c r="C214" s="21"/>
       <c r="D214" s="22"/>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" s="20"/>
       <c r="B215" s="20"/>
       <c r="C215" s="21"/>
       <c r="D215" s="22"/>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" s="20"/>
       <c r="B216" s="20"/>
       <c r="C216" s="21"/>
       <c r="D216" s="22"/>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" s="20"/>
       <c r="B217" s="20"/>
       <c r="C217" s="21"/>
       <c r="D217" s="22"/>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" s="20"/>
       <c r="B218" s="20"/>
       <c r="C218" s="21"/>
       <c r="D218" s="22"/>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" s="20"/>
       <c r="B219" s="20"/>
       <c r="C219" s="21"/>
       <c r="D219" s="22"/>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" s="20"/>
       <c r="B220" s="20"/>
       <c r="C220" s="21"/>
       <c r="D220" s="22"/>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" s="20"/>
       <c r="B221" s="20"/>
       <c r="C221" s="21"/>
       <c r="D221" s="22"/>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" s="20"/>
       <c r="B222" s="20"/>
       <c r="C222" s="21"/>
       <c r="D222" s="22"/>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" s="20"/>
       <c r="B223" s="20"/>
       <c r="C223" s="21"/>
       <c r="D223" s="22"/>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" s="20"/>
       <c r="B224" s="20"/>
       <c r="C224" s="21"/>
       <c r="D224" s="22"/>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" s="20"/>
       <c r="B225" s="20"/>
       <c r="C225" s="21"/>
       <c r="D225" s="22"/>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" s="20"/>
       <c r="B226" s="20"/>
       <c r="C226" s="21"/>
       <c r="D226" s="22"/>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" s="20"/>
       <c r="B227" s="20"/>
       <c r="C227" s="21"/>
       <c r="D227" s="22"/>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" s="20"/>
       <c r="B228" s="20"/>
       <c r="C228" s="21"/>
       <c r="D228" s="22"/>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" s="20"/>
       <c r="B229" s="20"/>
       <c r="C229" s="21"/>
       <c r="D229" s="22"/>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" s="20"/>
       <c r="B230" s="20"/>
       <c r="C230" s="21"/>
       <c r="D230" s="22"/>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" s="20"/>
       <c r="B231" s="20"/>
       <c r="C231" s="21"/>
       <c r="D231" s="22"/>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" s="20"/>
       <c r="B232" s="20"/>
       <c r="C232" s="21"/>
       <c r="D232" s="22"/>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" s="20"/>
       <c r="B233" s="20"/>
       <c r="C233" s="21"/>
       <c r="D233" s="22"/>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" s="20"/>
       <c r="B234" s="20"/>
       <c r="C234" s="21"/>
       <c r="D234" s="22"/>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" s="20"/>
       <c r="B235" s="20"/>
       <c r="C235" s="21"/>
       <c r="D235" s="22"/>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" s="20"/>
       <c r="B236" s="20"/>
       <c r="C236" s="21"/>
       <c r="D236" s="22"/>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" s="20"/>
       <c r="B237" s="20"/>
       <c r="C237" s="21"/>
       <c r="D237" s="22"/>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" s="20"/>
       <c r="B238" s="20"/>
       <c r="C238" s="21"/>
       <c r="D238" s="22"/>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" s="20"/>
       <c r="B239" s="20"/>
       <c r="C239" s="21"/>
       <c r="D239" s="22"/>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" s="20"/>
       <c r="B240" s="20"/>
       <c r="C240" s="21"/>
       <c r="D240" s="22"/>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" s="20"/>
       <c r="B241" s="20"/>
       <c r="C241" s="21"/>
       <c r="D241" s="22"/>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" s="20"/>
       <c r="B242" s="20"/>
       <c r="C242" s="21"/>
       <c r="D242" s="22"/>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" s="20"/>
       <c r="B243" s="20"/>
       <c r="C243" s="21"/>
       <c r="D243" s="22"/>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" s="20"/>
       <c r="B244" s="20"/>
       <c r="C244" s="21"/>
       <c r="D244" s="22"/>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" s="20"/>
       <c r="B245" s="20"/>
       <c r="C245" s="21"/>
       <c r="D245" s="22"/>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" s="20"/>
       <c r="B246" s="20"/>
       <c r="C246" s="21"/>
       <c r="D246" s="22"/>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" s="20"/>
       <c r="B247" s="20"/>
       <c r="C247" s="21"/>
       <c r="D247" s="22"/>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" s="20"/>
       <c r="B248" s="20"/>
       <c r="C248" s="21"/>
@@ -9436,12 +9436,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A86:A88"/>
-    <mergeCell ref="F37:F42"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="A84:A85"/>
     <mergeCell ref="A27:A30"/>
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="A43:A46"/>
@@ -9449,6 +9443,12 @@
     <mergeCell ref="A52:A55"/>
     <mergeCell ref="A56:A59"/>
     <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A86:A88"/>
+    <mergeCell ref="F37:F42"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="A84:A85"/>
   </mergeCells>
   <dataValidations count="20">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10 E18 E35" xr:uid="{FEC1871F-0B63-45CE-84E2-697ABFCCA571}">

</xml_diff>

<commit_message>
Fixed bugs in morphology updates
</commit_message>
<xml_diff>
--- a/docs/source/tutorials/GenVeg/GenVeg_Dune_Simulation.xlsx
+++ b/docs/source/tutorials/GenVeg/GenVeg_Dune_Simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\landlab\docs\source\tutorials\GenVeg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A97EA2-0021-47E8-B9D0-C71D22749FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E502BE08-2572-410A-B882-616C3FB5D314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
   </bookViews>
@@ -1582,8 +1582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59430052-850A-4E52-8B29-0C7825B169C3}">
   <dimension ref="A1:K264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5709,6 +5709,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A45:A51"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A36:A39"/>
     <mergeCell ref="A96:A97"/>
     <mergeCell ref="A99:A100"/>
     <mergeCell ref="A102:A104"/>
@@ -5719,16 +5729,6 @@
     <mergeCell ref="A87:A89"/>
     <mergeCell ref="A90:A92"/>
     <mergeCell ref="A93:A95"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A45:A51"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A36:A39"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="21">
@@ -9918,12 +9918,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A91:A93"/>
-    <mergeCell ref="F42:F47"/>
-    <mergeCell ref="A42:A47"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="A87:A88"/>
-    <mergeCell ref="A89:A90"/>
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="A48:A51"/>
@@ -9932,6 +9926,12 @@
     <mergeCell ref="A61:A64"/>
     <mergeCell ref="A65:A68"/>
     <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A91:A93"/>
+    <mergeCell ref="F42:F47"/>
+    <mergeCell ref="A42:A47"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A87:A88"/>
+    <mergeCell ref="A89:A90"/>
   </mergeCells>
   <dataValidations count="21">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11 E19 E40" xr:uid="{FEC1871F-0B63-45CE-84E2-697ABFCCA571}">

</xml_diff>